<commit_message>
Semana 10: Segundo grado
</commit_message>
<xml_diff>
--- a/santillana-recursos/semana_10/LGS1_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
+++ b/santillana-recursos/semana_10/LGS1_Aprende en casa_GAVI_Semana 10_2021-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fceron/Desktop/APRENDE EN CASA/SEMANA 10/DEFINITIVOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos.ciddelapaz/Library/Mobile Documents/com~apple~CloudDocs/Dev/GitHub/gavi/santillana-recursos/semana_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA08C6DE-CB92-4A42-9B0B-21542FFF17D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD40181E-C1DB-B641-8005-F06F773592A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="600" windowWidth="39420" windowHeight="25920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 10" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>La Guía Santillana 1. Aprende en casa_2021-2022. GAVI</t>
   </si>
@@ -291,9 +291,6 @@
       </rPr>
       <t>[Activación física]</t>
     </r>
-  </si>
-  <si>
-    <t>Páginas del libro de texto gratutito</t>
   </si>
   <si>
     <t>Martes 2 de noviembre</t>
@@ -1119,25 +1116,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="45">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1462,15 +1446,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1705,33 +1680,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1740,10 +1715,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1752,13 +1730,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1770,13 +1745,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1800,322 +1775,304 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2183,7 +2140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2235,7 +2192,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2438,61 +2395,61 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="D27" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
-    <col min="5" max="5" width="38.875" customWidth="1"/>
-    <col min="6" max="6" width="30.625" customWidth="1"/>
-    <col min="7" max="7" width="32.125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="38.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:8" ht="34" customHeight="1">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-    </row>
-    <row r="2" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A2" s="117" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+    </row>
+    <row r="2" spans="1:8" ht="32" customHeight="1">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="133"/>
-    </row>
-    <row r="4" spans="1:8" ht="37.35" customHeight="1">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="105"/>
+    </row>
+    <row r="4" spans="1:8" ht="37.25" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -2518,8 +2475,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="53.45" customHeight="1">
-      <c r="A5" s="106" t="s">
+    <row r="5" spans="1:8" ht="53.5" customHeight="1">
+      <c r="A5" s="90" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="36" t="s">
@@ -2543,7 +2500,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="54" customHeight="1">
-      <c r="A6" s="136"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2565,7 +2522,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="87" customHeight="1">
-      <c r="A7" s="136"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2586,40 +2543,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.7" customHeight="1">
-      <c r="A8" s="136"/>
-      <c r="B8" s="106" t="s">
+    <row r="8" spans="1:8" ht="43.75" customHeight="1">
+      <c r="A8" s="107"/>
+      <c r="B8" s="90" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="88"/>
-      <c r="H8" s="90" t="s">
+      <c r="G8" s="128"/>
+      <c r="H8" s="130" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.600000000000001" customHeight="1">
-      <c r="A9" s="136"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="137"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="91"/>
-    </row>
-    <row r="10" spans="1:8" ht="101.45" customHeight="1">
-      <c r="A10" s="107"/>
+    <row r="9" spans="1:8" ht="18.5" customHeight="1">
+      <c r="A9" s="107"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="125"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="131"/>
+    </row>
+    <row r="10" spans="1:8" ht="101.5" customHeight="1">
+      <c r="A10" s="91"/>
       <c r="B10" s="10" t="s">
         <v>28</v>
       </c>
@@ -2640,1076 +2597,897 @@
       </c>
       <c r="H10" s="55"/>
     </row>
-    <row r="11" spans="1:8" ht="18.95" customHeight="1">
-      <c r="A11" s="134"/>
-      <c r="B11" s="135"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="135"/>
-    </row>
-    <row r="12" spans="1:8" ht="32.450000000000003" customHeight="1">
-      <c r="A12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="15" t="s">
+    <row r="11" spans="1:8" ht="49.75" customHeight="1">
+      <c r="A11" s="106" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="49.7" customHeight="1">
-      <c r="A13" s="99" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="51"/>
+      <c r="H11" s="71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="72.5" customHeight="1">
+      <c r="A12" s="106"/>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="H12" s="71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="55.25" customHeight="1">
+      <c r="A13" s="106"/>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="68" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="51"/>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="72"/>
       <c r="H13" s="71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="72.599999999999994" customHeight="1">
-      <c r="A14" s="99"/>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="63" customHeight="1">
+      <c r="A14" s="106"/>
+      <c r="B14" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="53"/>
+      <c r="E14" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="54"/>
       <c r="H14" s="71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="55.35" customHeight="1">
-      <c r="A15" s="99"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="66.5" customHeight="1">
+      <c r="A15" s="106"/>
       <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="77"/>
+      <c r="H15" s="56"/>
+    </row>
+    <row r="16" spans="1:8" ht="80" customHeight="1">
+      <c r="A16" s="106" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="51"/>
+      <c r="H16" s="71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72" customHeight="1">
+      <c r="A17" s="106"/>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="85.25" customHeight="1">
+      <c r="A18" s="106"/>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="71" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="63" customHeight="1">
-      <c r="A16" s="99"/>
-      <c r="B16" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="E18" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="57"/>
+      <c r="H18" s="79" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="49.25" customHeight="1">
+      <c r="A19" s="106"/>
+      <c r="B19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="71" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="66.599999999999994" customHeight="1">
-      <c r="A17" s="99"/>
-      <c r="B17" s="1" t="s">
+      <c r="D19" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="60"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.5" customHeight="1">
+      <c r="A20" s="106"/>
+      <c r="B20" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="121" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="101"/>
+      <c r="H20" s="88" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="67.75" customHeight="1">
+      <c r="A21" s="106"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="89"/>
+    </row>
+    <row r="22" spans="1:8" ht="61.75" customHeight="1">
+      <c r="A22" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+    </row>
+    <row r="23" spans="1:8" ht="52.25" customHeight="1">
+      <c r="A23" s="106"/>
+      <c r="B23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="51"/>
+      <c r="H23" s="52"/>
+    </row>
+    <row r="24" spans="1:8" ht="70.75" customHeight="1">
+      <c r="A24" s="106"/>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="51"/>
+      <c r="H24" s="71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="61.75" customHeight="1">
+      <c r="A25" s="106"/>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="81"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="71"/>
+    </row>
+    <row r="26" spans="1:8" ht="50" customHeight="1">
+      <c r="A26" s="106"/>
+      <c r="B26" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="E26" s="83" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="99"/>
+      <c r="H26" s="119"/>
+    </row>
+    <row r="27" spans="1:8" ht="29.5" customHeight="1">
+      <c r="A27" s="106"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="120"/>
+    </row>
+    <row r="28" spans="1:8" ht="46.75" customHeight="1">
+      <c r="A28" s="116" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="G28" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" s="73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="63.5" customHeight="1">
+      <c r="A29" s="117"/>
+      <c r="B29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="51"/>
+      <c r="H29" s="71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="72.5" customHeight="1">
+      <c r="A30" s="117"/>
+      <c r="B30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="61"/>
+      <c r="G30" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="H30" s="62"/>
+    </row>
+    <row r="31" spans="1:8" ht="51" customHeight="1">
+      <c r="A31" s="117"/>
+      <c r="B31" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="63"/>
+      <c r="H31" s="64"/>
+    </row>
+    <row r="32" spans="1:8" ht="107.5" customHeight="1">
+      <c r="A32" s="118"/>
+      <c r="B32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="77"/>
-      <c r="H17" s="56"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="93"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="95"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-    </row>
-    <row r="20" spans="1:8" ht="34.700000000000003" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="80.099999999999994" customHeight="1">
-      <c r="A21" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="72" customHeight="1">
-      <c r="A22" s="99"/>
-      <c r="B22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="71" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="85.35" customHeight="1">
-      <c r="A23" s="99"/>
-      <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="57"/>
-      <c r="H23" s="79" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="49.35" customHeight="1">
-      <c r="A24" s="99"/>
-      <c r="B24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.6" customHeight="1">
-      <c r="A25" s="99"/>
-      <c r="B25" s="106" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="108" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="82" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="84" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="104" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="129"/>
-      <c r="H25" s="121" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="67.7" customHeight="1">
-      <c r="A26" s="99"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="110"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="105"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="100"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="101"/>
-      <c r="B28" s="101"/>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-    </row>
-    <row r="29" spans="1:8" ht="35.450000000000003" customHeight="1">
-      <c r="A29" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="61.7" customHeight="1">
-      <c r="A30" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" ht="52.35" customHeight="1">
-      <c r="A31" s="99"/>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
-    </row>
-    <row r="32" spans="1:8" ht="70.7" customHeight="1">
-      <c r="A32" s="99"/>
-      <c r="B32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" s="51"/>
-      <c r="H32" s="71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="61.7" customHeight="1">
-      <c r="A33" s="99"/>
-      <c r="B33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" s="81"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="71"/>
-    </row>
-    <row r="34" spans="1:11" ht="50.1" customHeight="1">
-      <c r="A34" s="99"/>
-      <c r="B34" s="106" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="122" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="123" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="124" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="125" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="127"/>
-      <c r="H34" s="102"/>
-    </row>
-    <row r="35" spans="1:11" ht="29.45" customHeight="1">
-      <c r="A35" s="99"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="126"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="103"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="92"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
+      <c r="D32" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="65"/>
+    </row>
+    <row r="33" spans="1:11" ht="43" customHeight="1">
+      <c r="A33" s="25"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="115"/>
+      <c r="G33" s="115"/>
+      <c r="H33" s="115"/>
+      <c r="K33" s="11"/>
+    </row>
+    <row r="34" spans="1:11" ht="63" customHeight="1">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="1:11" ht="72" customHeight="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:11" ht="64" customHeight="1">
+      <c r="A36" s="19"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="94"/>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
-      <c r="E37" s="95"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-    </row>
-    <row r="38" spans="1:11" ht="32.1">
-      <c r="A38" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="46.7" customHeight="1">
-      <c r="A39" s="96" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="74" t="s">
-        <v>95</v>
-      </c>
-      <c r="H39" s="73" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="63.6" customHeight="1">
-      <c r="A40" s="97"/>
-      <c r="B40" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40" s="51"/>
-      <c r="H40" s="71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="72.599999999999994" customHeight="1">
-      <c r="A41" s="97"/>
-      <c r="B41" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="61"/>
-      <c r="G41" s="74" t="s">
-        <v>101</v>
-      </c>
-      <c r="H41" s="62"/>
-    </row>
-    <row r="42" spans="1:11" ht="51" customHeight="1">
-      <c r="A42" s="97"/>
-      <c r="B42" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="63"/>
-      <c r="H42" s="64"/>
-    </row>
-    <row r="43" spans="1:11" ht="107.45" customHeight="1">
-      <c r="A43" s="98"/>
-      <c r="B43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H43" s="65"/>
-    </row>
-    <row r="44" spans="1:11" ht="42.95" customHeight="1">
-      <c r="A44" s="25"/>
-      <c r="B44" s="112"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="112"/>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="45" spans="1:11" ht="63" customHeight="1">
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30"/>
+    </row>
+    <row r="38" spans="1:11" ht="57" customHeight="1">
+      <c r="A38" s="112"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="114"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
+      <c r="H38" s="111"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="112"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="114"/>
+      <c r="F39" s="110"/>
+      <c r="G39" s="110"/>
+      <c r="H39" s="111"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="112"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="112"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+    </row>
+    <row r="42" spans="1:11" ht="50" customHeight="1">
+      <c r="A42" s="112"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+    </row>
+    <row r="43" spans="1:11" ht="83" customHeight="1">
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:11" ht="92" customHeight="1">
+      <c r="A44" s="19"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="20"/>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-    </row>
-    <row r="46" spans="1:11" ht="72" customHeight="1">
-      <c r="A46" s="21"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:11" ht="63.95" customHeight="1">
-      <c r="A47" s="19"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="20"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="30"/>
+    </row>
+    <row r="46" spans="1:11" ht="43" customHeight="1">
+      <c r="A46" s="112"/>
+      <c r="B46" s="113"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="111"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="112"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="113"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="110"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="111"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="30"/>
-    </row>
-    <row r="49" spans="1:8" ht="57" customHeight="1">
-      <c r="A49" s="113"/>
-      <c r="B49" s="113"/>
-      <c r="C49" s="93"/>
-      <c r="D49" s="113"/>
-      <c r="E49" s="114"/>
-      <c r="F49" s="115"/>
-      <c r="G49" s="115"/>
-      <c r="H49" s="116"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="113"/>
-      <c r="B50" s="113"/>
-      <c r="C50" s="93"/>
-      <c r="D50" s="113"/>
-      <c r="E50" s="114"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="116"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="113"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="113"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-    </row>
-    <row r="53" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A53" s="113"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-    </row>
-    <row r="54" spans="1:8" ht="83.1" customHeight="1">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="10"/>
-    </row>
-    <row r="55" spans="1:8" ht="92.1" customHeight="1">
-      <c r="A55" s="19"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="20"/>
+      <c r="A48" s="112"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="112"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+    </row>
+    <row r="50" spans="1:8" ht="40" customHeight="1">
+      <c r="A50" s="112"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+    </row>
+    <row r="51" spans="1:8" ht="53" customHeight="1">
+      <c r="B51" s="20"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8" ht="81" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="20"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="21"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="30"/>
+    </row>
+    <row r="54" spans="1:8" ht="64" customHeight="1">
+      <c r="A54" s="112"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="113"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="110"/>
+      <c r="G54" s="110"/>
+      <c r="H54" s="111"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="112"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="113"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="110"/>
+      <c r="G55" s="110"/>
+      <c r="H55" s="111"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="21"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="30"/>
-    </row>
-    <row r="57" spans="1:8" ht="42.95" customHeight="1">
-      <c r="A57" s="113"/>
-      <c r="B57" s="93"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="113"/>
-      <c r="E57" s="114"/>
-      <c r="F57" s="115"/>
-      <c r="G57" s="115"/>
-      <c r="H57" s="116"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="113"/>
-      <c r="B58" s="93"/>
-      <c r="C58" s="93"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="114"/>
-      <c r="F58" s="115"/>
-      <c r="G58" s="115"/>
-      <c r="H58" s="116"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="113"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="113"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-    </row>
-    <row r="61" spans="1:8" ht="39.950000000000003" customHeight="1">
-      <c r="A61" s="113"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" ht="53.1" customHeight="1">
-      <c r="B62" s="20"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="10"/>
-    </row>
-    <row r="63" spans="1:8" ht="81" customHeight="1">
-      <c r="A63" s="19"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="28"/>
-      <c r="H63" s="20"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="21"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="28"/>
-      <c r="H64" s="30"/>
-    </row>
-    <row r="65" spans="1:8" ht="63.95" customHeight="1">
-      <c r="A65" s="113"/>
-      <c r="B65" s="113"/>
-      <c r="C65" s="93"/>
-      <c r="D65" s="113"/>
-      <c r="E65" s="114"/>
-      <c r="F65" s="115"/>
-      <c r="G65" s="115"/>
-      <c r="H65" s="116"/>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="113"/>
-      <c r="B66" s="113"/>
-      <c r="C66" s="93"/>
-      <c r="D66" s="113"/>
-      <c r="E66" s="114"/>
-      <c r="F66" s="115"/>
-      <c r="G66" s="115"/>
-      <c r="H66" s="116"/>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="113"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="113"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-    </row>
-    <row r="69" spans="1:8" ht="74.099999999999994" customHeight="1">
-      <c r="A69" s="113"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-    </row>
-    <row r="70" spans="1:8" ht="45" customHeight="1">
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="10"/>
-    </row>
-    <row r="71" spans="1:8" ht="15.95" customHeight="1">
-      <c r="A71" s="19"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="20"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="21"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="30"/>
-    </row>
-    <row r="73" spans="1:8" ht="83.1" customHeight="1">
-      <c r="A73" s="113"/>
-      <c r="B73" s="93"/>
-      <c r="C73" s="93"/>
-      <c r="D73" s="113"/>
-      <c r="E73" s="114"/>
-      <c r="F73" s="115"/>
-      <c r="G73" s="115"/>
-      <c r="H73" s="116"/>
+      <c r="A56" s="112"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="112"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="1:8" ht="74" customHeight="1">
+      <c r="A58" s="112"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" ht="45" customHeight="1">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8" ht="16" customHeight="1">
+      <c r="A60" s="19"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="20"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="21"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="30"/>
+    </row>
+    <row r="62" spans="1:8" ht="83" customHeight="1">
+      <c r="A62" s="112"/>
+      <c r="B62" s="113"/>
+      <c r="C62" s="113"/>
+      <c r="D62" s="112"/>
+      <c r="E62" s="114"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="111"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="112"/>
+      <c r="B63" s="113"/>
+      <c r="C63" s="113"/>
+      <c r="D63" s="112"/>
+      <c r="E63" s="114"/>
+      <c r="F63" s="110"/>
+      <c r="G63" s="110"/>
+      <c r="H63" s="111"/>
+    </row>
+    <row r="64" spans="1:8" ht="16" customHeight="1">
+      <c r="A64" s="112"/>
+    </row>
+    <row r="65" spans="1:8" ht="36" customHeight="1">
+      <c r="A65" s="112"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+    </row>
+    <row r="66" spans="1:8" ht="86" customHeight="1">
+      <c r="A66" s="112"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+    </row>
+    <row r="67" spans="1:8" ht="113" customHeight="1">
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" ht="74" customHeight="1">
+      <c r="A68" s="19"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="28"/>
+      <c r="H68" s="10"/>
+    </row>
+    <row r="69" spans="1:8" ht="61" customHeight="1">
+      <c r="A69" s="21"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="30"/>
+    </row>
+    <row r="70" spans="1:8" ht="29" customHeight="1">
+      <c r="A70" s="112"/>
+      <c r="B70" s="112"/>
+      <c r="C70" s="113"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="114"/>
+      <c r="F70" s="110"/>
+      <c r="G70" s="110"/>
+      <c r="H70" s="111"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="112"/>
+      <c r="B71" s="112"/>
+      <c r="C71" s="113"/>
+      <c r="D71" s="112"/>
+      <c r="E71" s="114"/>
+      <c r="F71" s="110"/>
+      <c r="G71" s="110"/>
+      <c r="H71" s="111"/>
+    </row>
+    <row r="72" spans="1:8" ht="35" customHeight="1">
+      <c r="A72" s="112"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="112"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="113"/>
-      <c r="B74" s="93"/>
-      <c r="C74" s="93"/>
-      <c r="D74" s="113"/>
-      <c r="E74" s="114"/>
-      <c r="F74" s="115"/>
-      <c r="G74" s="115"/>
-      <c r="H74" s="116"/>
-    </row>
-    <row r="75" spans="1:8" ht="15.95" customHeight="1">
-      <c r="A75" s="113"/>
-    </row>
-    <row r="76" spans="1:8" ht="36" customHeight="1">
-      <c r="A76" s="113"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-    </row>
-    <row r="77" spans="1:8" ht="86.1" customHeight="1">
-      <c r="A77" s="113"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="21"/>
-    </row>
-    <row r="78" spans="1:8" ht="113.1" customHeight="1">
-      <c r="B78" s="10"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="28"/>
-      <c r="H78" s="10"/>
-    </row>
-    <row r="79" spans="1:8" ht="74.099999999999994" customHeight="1">
-      <c r="A79" s="19"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="28"/>
-      <c r="H79" s="10"/>
-    </row>
-    <row r="80" spans="1:8" ht="60.95" customHeight="1">
-      <c r="A80" s="21"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="28"/>
-      <c r="H80" s="30"/>
-    </row>
-    <row r="81" spans="1:8" ht="29.1" customHeight="1">
-      <c r="A81" s="113"/>
-      <c r="B81" s="113"/>
-      <c r="C81" s="93"/>
-      <c r="D81" s="113"/>
-      <c r="E81" s="114"/>
-      <c r="F81" s="115"/>
-      <c r="G81" s="115"/>
-      <c r="H81" s="116"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="113"/>
-      <c r="B82" s="113"/>
-      <c r="C82" s="93"/>
-      <c r="D82" s="113"/>
-      <c r="E82" s="114"/>
-      <c r="F82" s="115"/>
-      <c r="G82" s="115"/>
-      <c r="H82" s="116"/>
-    </row>
-    <row r="83" spans="1:8" ht="35.1" customHeight="1">
-      <c r="A83" s="113"/>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="113"/>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="113"/>
-    </row>
-    <row r="88" spans="1:8" ht="59.1" customHeight="1"/>
-    <row r="112" ht="53.1" customHeight="1"/>
-    <row r="113" ht="24.95" customHeight="1"/>
+      <c r="A74" s="112"/>
+    </row>
+    <row r="77" spans="1:8" ht="59" customHeight="1"/>
+    <row r="101" ht="53" customHeight="1"/>
+    <row r="102" ht="25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="A36:H37"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:H19"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A27:H28"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
+  <mergeCells count="69">
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>